<commit_message>
(CDV) Altered some stuff in loadgru_andtest vaali sheet.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -7,6 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mggB3JINfcFLV/iAFh4OvpxOHhTmQ=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -100,16 +105,16 @@
     <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1200</t>
   </si>
   <si>
+    <t>rnn_006</t>
+  </si>
+  <si>
+    <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std</t>
+  </si>
+  <si>
     <t>colab</t>
   </si>
   <si>
     <t>rnn_007</t>
-  </si>
-  <si>
-    <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std</t>
-  </si>
-  <si>
-    <t>rnn_006</t>
   </si>
   <si>
     <t>rnn_008</t>
@@ -133,12 +138,10 @@
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,14 +163,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -382,14 +381,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="6" width="12.63"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -418,7 +420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -447,7 +449,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -473,7 +476,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
@@ -499,7 +503,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9">
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -525,7 +530,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
@@ -551,7 +557,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -580,15 +587,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15">
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>24</v>
@@ -597,27 +605,28 @@
         <v>17</v>
       </c>
       <c r="F15" s="3">
-        <v>30.0</v>
+        <v>150.0</v>
       </c>
       <c r="G15" s="3">
-        <v>30.0</v>
+        <v>150.0</v>
       </c>
       <c r="H15" s="3">
         <v>0.1</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -626,21 +635,22 @@
         <v>17</v>
       </c>
       <c r="F17" s="3">
-        <v>150.0</v>
+        <v>30.0</v>
       </c>
       <c r="G17" s="3">
-        <v>150.0</v>
+        <v>30.0</v>
       </c>
       <c r="H17" s="3">
         <v>0.1</v>
       </c>
       <c r="I17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>33</v>
@@ -667,6 +677,987 @@
         <v>34</v>
       </c>
     </row>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
(CDV) trained rnn_009, minor edits to other files.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>RNN</t>
   </si>
@@ -108,19 +108,25 @@
     <t>rnn_006</t>
   </si>
   <si>
+    <t>colab</t>
+  </si>
+  <si>
+    <t>rnn_007</t>
+  </si>
+  <si>
     <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std</t>
   </si>
   <si>
-    <t>colab</t>
-  </si>
-  <si>
-    <t>rnn_007</t>
-  </si>
-  <si>
     <t>rnn_008</t>
   </si>
   <si>
     <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
+  </si>
+  <si>
+    <t>rnn_009</t>
+  </si>
+  <si>
+    <t>random uniform noise (stddev=1e-4) added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -167,6 +173,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -613,17 +622,17 @@
       <c r="H15" s="3">
         <v>0.1</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>30</v>
+      <c r="I15" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>12</v>
@@ -644,13 +653,13 @@
         <v>0.1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>33</v>
@@ -678,7 +687,35 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
(CDV) Trained rnn_010, minor edits to other files.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>RNN</t>
   </si>
@@ -108,6 +108,9 @@
     <t>rnn_006</t>
   </si>
   <si>
+    <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
+  </si>
+  <si>
     <t>colab</t>
   </si>
   <si>
@@ -120,13 +123,16 @@
     <t>rnn_008</t>
   </si>
   <si>
-    <t>random uniform noise added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
-  </si>
-  <si>
     <t>rnn_009</t>
   </si>
   <si>
     <t>random uniform noise (stddev=1e-4) added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
+  </si>
+  <si>
+    <t>rnn_010</t>
+  </si>
+  <si>
+    <t>random uniform noise (stddev=1e-3) added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, Tsim=1000</t>
   </si>
 </sst>
 </file>
@@ -623,16 +629,16 @@
         <v>0.1</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>12</v>
@@ -653,16 +659,16 @@
         <v>0.1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>20</v>
@@ -683,13 +689,13 @@
         <v>0.1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>35</v>
@@ -717,7 +723,35 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
(KS) Computed difference in hidden states of teacher-forced and AR GRU.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="82">
   <si>
     <t>RNN</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>ae_013</t>
+  </si>
+  <si>
+    <t>ae_015</t>
+  </si>
+  <si>
+    <t>data_002</t>
   </si>
 </sst>
 </file>
@@ -2450,6 +2456,29 @@
         <v>53</v>
       </c>
     </row>
+    <row r="33">
+      <c r="B33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
(KS) Modified MakeData.ipynb to save lp spectrum and other stuff properly. Added GRU template that makes use of P1@phi+P2@phi^2. Modified RNN training to properly account for validation datasets.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -17,11 +17,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="89">
   <si>
     <t>RNN</t>
   </si>
   <si>
+    <t>GRU and LSTM v3 are for the case where the input to the RNN during training was normalized but the output was not</t>
+  </si>
+  <si>
     <t>Folder</t>
   </si>
   <si>
@@ -205,6 +208,15 @@
     <t>ae_004</t>
   </si>
   <si>
+    <t>LR sigmoid (warmup 40, expected 100)</t>
+  </si>
+  <si>
+    <t>3*meanLpTime</t>
+  </si>
+  <si>
+    <t>random uniform noise (fRMS=0.05) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6</t>
+  </si>
+  <si>
     <t>ae_005</t>
   </si>
   <si>
@@ -214,9 +226,15 @@
     <t>[24, 32, 48, 64, 96, 128]</t>
   </si>
   <si>
+    <t>random uniform noise (fRMS=0.05) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v7</t>
+  </si>
+  <si>
     <t>ae_006</t>
   </si>
   <si>
+    <t>[256]</t>
+  </si>
+  <si>
     <t>ae_007</t>
   </si>
   <si>
@@ -227,6 +245,9 @@
   </si>
   <si>
     <t>ae_008</t>
+  </si>
+  <si>
+    <t>LR sigmoid (warmup 10, expected 25)</t>
   </si>
   <si>
     <t>ae_009</t>
@@ -283,17 +304,17 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -320,22 +341,22 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -565,351 +586,354 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3">
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4">
         <v>30.0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>30.0</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>0.1</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4">
         <v>30.0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>30.0</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>0.1</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>18</v>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4">
+        <v>60.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>60.0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4">
         <v>60.0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
         <v>60.0</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>0.1</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>22</v>
+      <c r="I9" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4">
+        <v>60.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>60.0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4">
         <v>90.0</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="4">
         <v>90.0</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>0.1</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>28</v>
+      <c r="I13" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="E15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="4">
+        <v>150.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>150.0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="3">
-        <v>150.0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>150.0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="4">
         <v>30.0</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="4">
         <v>30.0</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>0.1</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>32</v>
+      <c r="I17" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="4">
         <v>90.0</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="4">
         <v>90.0</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>0.1</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>34</v>
+      <c r="I19" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="4">
         <v>90.0</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="4">
         <v>90.0</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>0.1</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>36</v>
+      <c r="I21" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="A23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="4">
         <v>90.0</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="4">
         <v>90.0</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>0.1</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>38</v>
+      <c r="I23" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -1911,102 +1935,102 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>39</v>
+      <c r="A1" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>9</v>
+      <c r="U2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="6">
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="2">
         <v>48.0</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>10</v>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="R3" s="7">
         <v>10.0</v>
@@ -2014,46 +2038,49 @@
       <c r="S3" s="7">
         <v>10.0</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="4">
         <v>0.1</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="6">
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="2">
         <v>48.0</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="N5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="R5" s="7">
         <v>10.0</v>
@@ -2061,43 +2088,43 @@
       <c r="S5" s="7">
         <v>10.0</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="4">
         <v>0.1</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6">
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2">
         <v>32.0</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>49</v>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="R7" s="7">
         <v>10.0</v>
@@ -2105,43 +2132,43 @@
       <c r="S7" s="7">
         <v>10.0</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="4">
         <v>0.1</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="D9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2">
         <v>24.0</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>49</v>
+      <c r="G9" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="R9" s="7">
         <v>10.0</v>
@@ -2149,334 +2176,414 @@
       <c r="S9" s="7">
         <v>10.0</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="4">
         <v>0.1</v>
       </c>
       <c r="U9" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2">
+        <v>32.0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="E15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="H15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="R15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="S15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T15" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T17" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2">
         <v>16.0</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T19" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="6">
-        <v>24.0</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="F21" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="H23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="E33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="F33" s="2">
         <v>16.0</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>53</v>
+      <c r="G33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(KS) Trained rnn_009 and rnn_010, fixed normalizatio_arr error in prediction horizon notebook.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="92">
   <si>
     <t xml:space="preserve">RNN</t>
   </si>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">[8, 16, 24, 32, 48, 64, 96, 128]</t>
   </si>
   <si>
-    <t xml:space="preserve">random uniform noise (fRMS=0.00) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 2000 max epochs, 50 patience, 1e-6 min error dif; GRU_SingleStep_v6</t>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6</t>
   </si>
   <si>
     <t xml:space="preserve">ae_010</t>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t xml:space="preserve">[512]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6</t>
   </si>
   <si>
     <t xml:space="preserve">ae_011</t>
@@ -1797,7 +1794,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y5" activeCellId="0" sqref="Y5"/>
+      <selection pane="topLeft" activeCell="U23" activeCellId="0" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2330,7 +2327,7 @@
         <v>25</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>64</v>
@@ -2390,18 +2387,18 @@
         <v>0.1</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>49</v>
@@ -2415,7 +2412,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
@@ -2438,13 +2435,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>49</v>
@@ -2458,7 +2455,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
@@ -2481,7 +2478,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>67</v>
@@ -2496,7 +2493,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
(KS) Trained AR_rnn_003 and AR_rnn_004.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="93">
   <si>
     <t xml:space="preserve">RNN</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t xml:space="preserve">[4, 8, 16, 24, 32, 48, 64, 96, 128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_011</t>
   </si>
   <si>
     <t xml:space="preserve">ae_012</t>
@@ -1794,7 +1797,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U23" activeCellId="0" sqref="U23"/>
+      <selection pane="topLeft" activeCell="U25" activeCellId="0" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2390,7 +2393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
         <v>84</v>
       </c>
@@ -2409,10 +2412,34 @@
       <c r="G25" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="N25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
@@ -2435,7 +2462,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>85</v>
@@ -2455,7 +2482,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
@@ -2478,7 +2505,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>67</v>
@@ -2493,7 +2520,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
(KS) Added ESN training, both regular and residual. Trained rnn_012, rnn_013, rnn_014 and rnn_015.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="104">
   <si>
     <t xml:space="preserve">RNN</t>
   </si>
@@ -191,6 +191,9 @@
     <t xml:space="preserve">random uniform noise (std=1e-4) added to hidden states, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 20 patience, 5e-6 min error dif</t>
   </si>
   <si>
+    <t xml:space="preserve">residualPlus is not regular residual network, here the skip connection itself is multiplied with a weight matrix.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ae_002</t>
   </si>
   <si>
@@ -290,16 +293,46 @@
     <t xml:space="preserve">ae_012</t>
   </si>
   <si>
+    <t xml:space="preserve">rnn_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10*meanLpTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.0) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 25 patience, 5e-6 min error dif; connectivity=0.3 spectral_radius=0.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">ae_014</t>
   </si>
   <si>
+    <t xml:space="preserve">rnn_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.0) added to inputs, excluding the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 25 patience, 5e-6 min error dif; connectivity=0.1 spectral_radius=0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ae_013</t>
   </si>
   <si>
+    <t xml:space="preserve">rnn_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESN-residualPlus</t>
+  </si>
+  <si>
     <t xml:space="preserve">ae_015</t>
   </si>
   <si>
     <t xml:space="preserve">data_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random gaussian noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 25 patience, 5e-6 min error dif; degree=3 spectral_radius=0.6</t>
   </si>
 </sst>
 </file>
@@ -390,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,6 +442,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -434,7 +471,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1797,10 +1834,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U25" activeCellId="0" sqref="U25"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1979,9 +2016,14 @@
         <v>55</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>47</v>
@@ -2020,18 +2062,18 @@
         <v>0.1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>49</v>
@@ -2064,12 +2106,12 @@
         <v>0.1</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>47</v>
@@ -2099,30 +2141,30 @@
         <v>25</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T11" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>49</v>
@@ -2144,30 +2186,30 @@
         <v>25</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T13" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>49</v>
@@ -2186,36 +2228,36 @@
         <v>30</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T15" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>49</v>
@@ -2231,36 +2273,36 @@
         <v>32</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T17" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>49</v>
@@ -2279,36 +2321,36 @@
         <v>34</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T19" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>49</v>
@@ -2324,7 +2366,7 @@
         <v>36</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>25</v>
@@ -2333,27 +2375,27 @@
         <v>18</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T21" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>49</v>
@@ -2369,10 +2411,10 @@
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>25</v>
@@ -2381,27 +2423,27 @@
         <v>18</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T23" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>49</v>
@@ -2413,7 +2455,7 @@
         <v>50</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>28</v>
@@ -2425,27 +2467,27 @@
         <v>18</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T25" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="U25" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>49</v>
@@ -2459,16 +2501,40 @@
       <c r="H27" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>49</v>
@@ -2479,16 +2545,40 @@
       <c r="G29" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>49</v>
@@ -2502,16 +2592,40 @@
       <c r="H31" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>49</v>
@@ -2520,10 +2634,34 @@
         <v>16</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T33" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bunch of changes, now saving everything in rnns. Bunch of new rnns.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="134">
   <si>
     <t xml:space="preserve">RNN</t>
   </si>
@@ -333,6 +333,114 @@
   </si>
   <si>
     <t xml:space="preserve">random gaussian noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 25 patience, 5e-6 min error dif; degree=3 spectral_radius=0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRU (v6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5*meanLpTime</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">skip_intermediate=1/3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediat=1/3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRU (v?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[256, 246]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[256, 256]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnn_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no noise added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with minmax, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘sigmoid’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘relu’, ‘linear’], dense_dim=[512, 32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘relu’, ‘linear’], dense_dim=[256, 32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘sigmoid’, ‘linear’], dense_dim=[256, 32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[768]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘linear’], dense_dim=[32]</t>
   </si>
 </sst>
 </file>
@@ -342,7 +450,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -379,6 +487,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -440,12 +554,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -471,7 +585,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1831,26 +1945,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U37" activeCellId="0" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="4" width="12.7"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
       <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1980,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +2033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1966,7 +2083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
         <v>52</v>
       </c>
@@ -2017,11 +2134,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
         <v>57</v>
       </c>
@@ -2065,7 +2182,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
         <v>59</v>
       </c>
@@ -2109,7 +2226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
@@ -2156,7 +2273,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
@@ -2201,7 +2318,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
         <v>71</v>
       </c>
@@ -2249,7 +2366,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
         <v>73</v>
       </c>
@@ -2294,7 +2411,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
         <v>76</v>
       </c>
@@ -2662,6 +2779,491 @@
       </c>
       <c r="U33" s="2" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T35" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T41" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N43" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T43" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U43" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N45" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T45" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T47" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T49" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N51" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T51" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U51" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N53" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="P53" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T53" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U53" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N55" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P55" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T55" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N57" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P57" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T57" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N59" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P59" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T59" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U59" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P61" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T61" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U61" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P63" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T63" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U63" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P65" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q65" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R65" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S65" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T65" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U65" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P67" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R67" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T67" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U67" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N69" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P69" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q69" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R69" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S69" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T69" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U69" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N71" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O71" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P71" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T71" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U71" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bunch of changes, should've committed on the way *sigh*. Added contractive AE, learnt the lambda_reg was just too high. Fixed minor error in AR RNN training that was causing it to not load the weights. Computed new KS data (T=50000), can't data.npz to github because file size limit.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="192">
   <si>
     <t xml:space="preserve">RNN</t>
   </si>
@@ -335,6 +335,12 @@
     <t xml:space="preserve">random gaussian noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and std, 200 max epochs, 25 patience, 5e-6 min error dif; degree=3 spectral_radius=0.6</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_004</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_020</t>
   </si>
   <si>
@@ -344,103 +350,253 @@
     <t xml:space="preserve">5*meanLpTime</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">skip_intermediate=1/3</t>
-    </r>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_017</t>
   </si>
   <si>
     <t xml:space="preserve">rnn_021</t>
   </si>
   <si>
+    <t xml:space="preserve">GRU (v7)</t>
+  </si>
+  <si>
     <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediat=1/3</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_018</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_022</t>
   </si>
   <si>
     <t xml:space="preserve">?</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_019</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_023</t>
   </si>
   <si>
     <t xml:space="preserve">GRU (v?)</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_020</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_024</t>
   </si>
   <si>
-    <t xml:space="preserve">[256, 246]</t>
+    <t xml:space="preserve">[256, 256]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_021</t>
   </si>
   <si>
     <t xml:space="preserve">rnn_025</t>
   </si>
   <si>
-    <t xml:space="preserve">[256, 256]</t>
+    <t xml:space="preserve">ae_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_005</t>
   </si>
   <si>
     <t xml:space="preserve">rnn_026</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[128, 96, 64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[64, 96, 128]</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_027</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_024</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_028</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_025</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_029</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_026</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_030</t>
   </si>
   <si>
     <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_027</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_031</t>
   </si>
   <si>
     <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev3, [tanh, tanh, tanh, linear]</t>
+  </si>
+  <si>
     <t xml:space="preserve">rnn_032</t>
   </si>
   <si>
     <t xml:space="preserve">no noise added to inputs, including the first timestep, dataset normalized (featurewise) with sample mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; GRU_SingleStep_v6, skip_intermediate=1/4</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [elu, tanh, elu, linear], fRMS=0.0025</t>
+  </si>
+  <si>
     <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with minmax, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘sigmoid’]</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev3, [relu, relu, relu, sigmoid], BinarCrossentropy loss, minmax scaling, ignoring params</t>
+  </si>
+  <si>
     <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘relu’, ‘linear’], dense_dim=[512, 32]</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [relu, tanh, relu, tanh], fRMS=0.01, ignoring params</t>
+  </si>
+  <si>
     <t xml:space="preserve">random normal noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘relu’, ‘linear’], dense_dim=[256, 32]</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [relu, tanh, relu, linear], fRMS=0.01, ignoring params, minmax normalization</t>
+  </si>
+  <si>
     <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 2000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘sigmoid’, ‘linear’], dense_dim=[256, 32]</t>
   </si>
   <si>
+    <t xml:space="preserve">ae_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [relu, tanh, relu, linear], fRMS=0.01, ignoring params, stddev normalization</t>
+  </si>
+  <si>
     <t xml:space="preserve">[768]</t>
   </si>
   <si>
     <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/4, dense_layer_act_func=[‘linear’], dense_dim=[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[192, 128, 96, 64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[64, 96, 128, 192]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev5, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization, contractive_lmda=0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRU (v8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/3, dense_layer_act_func=[‘linear’], dense_dim=[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev5, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization, contractive_lmda=10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev5, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization, contractive_lmda=50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[256, 256, 256]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=’full sample’, dense_layer_act_func=[‘linear’], dense_dim=[32], POD – data_dir 005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.025) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/2, aev5 used dense_layer_act_func=[‘linear’], dense_dim=[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev5, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization, contractive_lmda=50, reg_lmda=1e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.01) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/2, aev5 used dense_layer_act_func=[‘linear’], dense_dim=[48], lmda_reg=1e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aev4, [elu, tanh, elu, linear], fRMS=0.01, ignoring params, stddev normalization, reg_lmda=1e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.01) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/2, aev5 used dense_layer_act_func=[‘linear’], dense_dim=[16], lmda_reg=1e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random uniform noise (fRMS=0.005) added to inputs, including the first timestep, dataset normalized (featurewise) with mean and 3*std, 1000 max epochs, 25 patience, 1e-6 min error dif; skip_intermediate=1/2, aev5 used dense_layer_act_func=[‘linear’], dense_dim=[16], lmda_reg=1e-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae_047</t>
   </si>
 </sst>
 </file>
@@ -450,7 +606,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -487,12 +643,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -585,7 +735,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1945,10 +2095,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U37" activeCellId="0" sqref="U37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U90" activeCellId="0" sqref="U90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2782,335 +2932,593 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N35" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O35" s="4" t="s">
         <v>84</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T35" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N37" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O37" s="4" t="s">
         <v>72</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T37" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N39" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Q39" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T39" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N41" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="O41" s="4" t="s">
         <v>72</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T41" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N43" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T43" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N45" s="4" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P45" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T45" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N47" s="4" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="O47" s="4" t="s">
         <v>84</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T47" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N49" s="4" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="P49" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T49" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N51" s="4" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T51" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N53" s="4" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T53" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N55" s="4" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="O55" s="4" t="s">
         <v>84</v>
       </c>
       <c r="P55" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q55" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T55" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U55" s="2" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="N57" s="4" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>84</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q57" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R57" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T57" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U57" s="2" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="N59" s="4" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="O59" s="4" t="s">
         <v>84</v>
       </c>
       <c r="P59" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q59" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R59" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T59" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U59" s="2" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="N61" s="4" t="s">
         <v>12</v>
       </c>
@@ -3118,51 +3526,93 @@
         <v>84</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q61" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T61" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U61" s="2" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="N63" s="4" t="s">
         <v>17</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P63" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q63" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R63" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T63" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U63" s="2" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="N65" s="4" t="s">
         <v>20</v>
       </c>
@@ -3170,25 +3620,46 @@
         <v>84</v>
       </c>
       <c r="P65" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q65" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R65" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T65" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U65" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="N67" s="4" t="s">
         <v>22</v>
       </c>
@@ -3196,25 +3667,46 @@
         <v>72</v>
       </c>
       <c r="P67" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R67" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T67" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U67" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="N69" s="4" t="s">
         <v>24</v>
       </c>
@@ -3222,48 +3714,584 @@
         <v>72</v>
       </c>
       <c r="P69" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q69" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R69" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S69" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T69" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U69" s="2" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="N71" s="4" t="s">
         <v>27</v>
       </c>
       <c r="O71" s="4" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="P71" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q71" s="2" t="s">
         <v>49</v>
       </c>
       <c r="R71" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="T71" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="U71" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q73" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S73" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T73" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U73" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R75" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S75" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T75" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U75" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F77" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S77" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T77" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U77" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T79" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U79" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q81" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T81" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U81" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N83" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P83" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q83" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R83" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S83" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T83" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U83" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F85" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="N85" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O85" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P85" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q85" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R85" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S85" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T85" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U85" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F87" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R87" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T87" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U87" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F89" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O89" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T89" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U89" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F91" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F93" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F95" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F97" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bunch of changes. Wrote my own ESN classes, trained a bunch of them. Wrote ESNv3 that saves the sparse matrices as sparse matrices, thus saving a ton of space. Performed some grid searches for the ESNs - excellent results.
</commit_message>
<xml_diff>
--- a/File Tracking.xlsx
+++ b/File Tracking.xlsx
@@ -735,7 +735,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2097,7 +2097,7 @@
   </sheetPr>
   <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U90" activeCellId="0" sqref="U90"/>
     </sheetView>
   </sheetViews>

</xml_diff>